<commit_message>
Test - commit with file open
</commit_message>
<xml_diff>
--- a/Ionocyte/All 1dph ionocyte data.xlsx
+++ b/Ionocyte/All 1dph ionocyte data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82A8396E-9639-477A-B4EC-770FB7CE5CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E89A84-069F-43E1-A8B5-55D9B2C2230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="balanceddata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="416">
   <si>
     <t>Experiment</t>
   </si>
@@ -1265,12 +1265,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>testing whether you can commit with the file open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2105,11 +2108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2400,6 +2403,9 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Test save with file open after adding gitignore
</commit_message>
<xml_diff>
--- a/Ionocyte/All 1dph ionocyte data.xlsx
+++ b/Ionocyte/All 1dph ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4D989F-06D5-4EAA-B2A9-5A0DB8390D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC624A94-65F1-40CA-A1B8-108ACCB20F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="416">
   <si>
     <t>Experiment</t>
   </si>
@@ -1265,6 +1265,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>testing again with gitignore added</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2112,7 @@
   <dimension ref="A1:AE365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2400,6 +2403,9 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Fixed suspicious zero-ionocyte counts in embryo; fixed some larvae areas that were in wrong units
</commit_message>
<xml_diff>
--- a/Ionocyte/All 1dph ionocyte data.xlsx
+++ b/Ionocyte/All 1dph ionocyte data.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{14BCB123-1E69-456C-8116-F6DD8836333B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9B47EE-4D71-4B73-B196-25AD477CAA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp 1dph data with trmt levels" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1405,7 +1417,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2241,11 +2253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AY10" sqref="AY10"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2436,39 +2448,114 @@
       <c r="E2">
         <v>390262.16220000002</v>
       </c>
+      <c r="F2">
+        <f>E2/1000000</f>
+        <v>0.39026216220000004</v>
+      </c>
       <c r="G2">
         <v>81</v>
       </c>
       <c r="H2">
         <v>300265.11910000001</v>
       </c>
+      <c r="I2">
+        <f>H2/1000000</f>
+        <v>0.30026511910000003</v>
+      </c>
       <c r="J2">
         <v>61</v>
       </c>
       <c r="K2">
-        <v>2.07553E-4</v>
+        <f>G2/E2</f>
+        <v>2.0755278847271245E-4</v>
+      </c>
+      <c r="L2">
+        <f>G2/F2</f>
+        <v>207.55278847271245</v>
       </c>
       <c r="M2">
-        <v>2.0315399999999999E-4</v>
+        <f>J2/H2</f>
+        <v>2.0315380015780194E-4</v>
+      </c>
+      <c r="N2">
+        <f>J2/I2</f>
+        <v>203.15380015780192</v>
+      </c>
+      <c r="O2">
+        <f>E2+H2</f>
+        <v>690527.28130000003</v>
+      </c>
+      <c r="P2">
+        <f>F2+I2</f>
+        <v>0.69052728130000007</v>
+      </c>
+      <c r="Q2">
+        <f>G2+J2</f>
+        <v>142</v>
+      </c>
+      <c r="R2">
+        <f>Q2/O2</f>
+        <v>2.0563995637169909E-4</v>
+      </c>
+      <c r="S2">
+        <f>Q2/P2</f>
+        <v>205.6399563716991</v>
       </c>
       <c r="T2">
         <v>542369.82810000004</v>
       </c>
+      <c r="U2">
+        <f>T2/1000000</f>
+        <v>0.54236982810000001</v>
+      </c>
       <c r="V2">
         <v>32</v>
       </c>
       <c r="W2">
         <v>466419.66710000002</v>
       </c>
+      <c r="X2">
+        <f>W2/1000000</f>
+        <v>0.46641966710000005</v>
+      </c>
       <c r="Y2">
         <v>56</v>
       </c>
       <c r="Z2" s="1">
-        <v>5.8999999999999998E-5</v>
-      </c>
-      <c r="AA2" s="1"/>
+        <f>V2/T2</f>
+        <v>5.9000332138866626E-5</v>
+      </c>
+      <c r="AA2" s="1">
+        <f>V2/U2</f>
+        <v>59.000332138866632</v>
+      </c>
       <c r="AB2">
-        <v>1.2006399999999999E-4</v>
+        <f>Y2/W2</f>
+        <v>1.2006354780917428E-4</v>
+      </c>
+      <c r="AC2">
+        <f>Y2/X2</f>
+        <v>120.06354780917427</v>
+      </c>
+      <c r="AD2">
+        <f>T2+W2</f>
+        <v>1008789.4952</v>
+      </c>
+      <c r="AE2">
+        <f>U2+X2</f>
+        <v>1.0087894952000001</v>
+      </c>
+      <c r="AF2">
+        <f>V2+Y2</f>
+        <v>88</v>
+      </c>
+      <c r="AG2">
+        <f>AF2/AD2</f>
+        <v>8.7233263647886573E-5</v>
+      </c>
+      <c r="AH2">
+        <f>AF2/AE2</f>
+        <v>87.23326364788656</v>
       </c>
       <c r="AJ2" s="1"/>
     </row>
@@ -2505,7 +2592,7 @@
         <v>2.8593500000000002E-4</v>
       </c>
       <c r="T3">
-        <v>340228</v>
+        <v>302764.814464</v>
       </c>
       <c r="V3">
         <v>15</v>
@@ -2559,7 +2646,7 @@
         <v>2.4524200000000001E-4</v>
       </c>
       <c r="T4">
-        <v>407389</v>
+        <v>362530.58243200002</v>
       </c>
       <c r="V4">
         <v>23</v>
@@ -3332,7 +3419,7 @@
         <v>4.0068900000000003E-4</v>
       </c>
       <c r="T19">
-        <v>454772</v>
+        <v>404696.14553600003</v>
       </c>
       <c r="V19">
         <v>194</v>
@@ -3944,7 +4031,7 @@
         <v>3.8029399999999999E-4</v>
       </c>
       <c r="T31">
-        <v>329891</v>
+        <v>293566.04220800003</v>
       </c>
       <c r="V31">
         <v>164</v>

</xml_diff>